<commit_message>
job and assessment delete
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Akash\inertia\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4043548-8076-4EF1-8F87-4BFD16C2BF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1545D-68D3-4993-857D-F4FE1F797403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
   <si>
     <t>Question</t>
   </si>
@@ -253,9 +253,6 @@
   </si>
   <si>
     <t>Workplace Safety And Welfare</t>
-  </si>
-  <si>
-    <t>#640606</t>
   </si>
 </sst>
 </file>
@@ -633,7 +630,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>